<commit_message>
Import Client: Add Update client when found, and remove close button.
</commit_message>
<xml_diff>
--- a/ztestFiles/Excell001.xlsx
+++ b/ztestFiles/Excell001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hds\Billing\workspace\billingcv\ztestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EA58CBFC-20A7-4353-B0D1-EE10ED8C0730}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4A7CE07-A0DF-419F-91BF-8FF0DD2CF9DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{6124A34B-4CD8-4CDD-8E59-F39365CFC31A}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="fileClient001" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">fileClient001!$A$1:$H$18</definedName>
+    <definedName name="DadosExternos_1" localSheetId="0" hidden="1">fileClient001!$A$1:$H$87</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="173">
   <si>
     <t>Client</t>
   </si>
@@ -186,6 +186,384 @@
   </si>
   <si>
     <t>Infra Essentials</t>
+  </si>
+  <si>
+    <t>ACILNXLAB01</t>
+  </si>
+  <si>
+    <t>acilnxlab01.globosat.net.br</t>
+  </si>
+  <si>
+    <t>ACV-CONT-CLT-MN</t>
+  </si>
+  <si>
+    <t>WIN-4GKB4466MHU</t>
+  </si>
+  <si>
+    <t>ACV-CONT-SUP-1</t>
+  </si>
+  <si>
+    <t>ACV-CONT-SUP-1.eng.cpp</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-CORE1</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-CORE1.eng.cpp</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-CORE2</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-CORE2.eng.cpp</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-CORE3</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-CORE3.eng.cpp</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-DSB</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-GWEB</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-GWEB.eng.cpp</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-ING</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-ING.eng.cpp</t>
+  </si>
+  <si>
+    <t>acv-ctrl-kpi</t>
+  </si>
+  <si>
+    <t>10.228.136.75</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-WEB</t>
+  </si>
+  <si>
+    <t>ACV-CTRL-WEB.eng.cpp</t>
+  </si>
+  <si>
+    <t>AD1-VFX</t>
+  </si>
+  <si>
+    <t>AD1-VFX.vfx.eng.cpp</t>
+  </si>
+  <si>
+    <t>AD2-CPP</t>
+  </si>
+  <si>
+    <t>AD2-CPP.eng.cpp</t>
+  </si>
+  <si>
+    <t>ADBY-VFX</t>
+  </si>
+  <si>
+    <t>ADBY-VFX.vfx.eng.cpp</t>
+  </si>
+  <si>
+    <t>ANSIBLE</t>
+  </si>
+  <si>
+    <t>PVWSRV0000236</t>
+  </si>
+  <si>
+    <t>PVWSRV0000236.globosat.net.br</t>
+  </si>
+  <si>
+    <t>PVWSRV0000239</t>
+  </si>
+  <si>
+    <t>PVWSRV0000239.globosat.net.br</t>
+  </si>
+  <si>
+    <t>PVWSRV0000263</t>
+  </si>
+  <si>
+    <t>PVWSRV0000263.globosat.net.br</t>
+  </si>
+  <si>
+    <t>Servidor Físico</t>
+  </si>
+  <si>
+    <t>Cluster HyperV</t>
+  </si>
+  <si>
+    <t>rj2k8vcb01</t>
+  </si>
+  <si>
+    <t>10.1.0.24</t>
+  </si>
+  <si>
+    <t>RJ2K8VMREP01</t>
+  </si>
+  <si>
+    <t>rj2k8vmrep01.globosat.net.br</t>
+  </si>
+  <si>
+    <t>rj2k8vmrep01</t>
+  </si>
+  <si>
+    <t>10.1.0.150</t>
+  </si>
+  <si>
+    <t>clpabkpsr001</t>
+  </si>
+  <si>
+    <t>10.118.0.4</t>
+  </si>
+  <si>
+    <t>Azure Cloud</t>
+  </si>
+  <si>
+    <t>Gabriel Branco</t>
+  </si>
+  <si>
+    <t>backoffice.backup@g.globo</t>
+  </si>
+  <si>
+    <t>gabriel@g.globo</t>
+  </si>
+  <si>
+    <t>Backoffice Backup</t>
+  </si>
+  <si>
+    <t>clpabkpsr004</t>
+  </si>
+  <si>
+    <t>CLPABKPSR004</t>
+  </si>
+  <si>
+    <t>10.118.0.7</t>
+  </si>
+  <si>
+    <t>CLPABKPSR005</t>
+  </si>
+  <si>
+    <t>clpabkpsr005</t>
+  </si>
+  <si>
+    <t>10.116.0.4</t>
+  </si>
+  <si>
+    <t>clpabkpsr006</t>
+  </si>
+  <si>
+    <t>CLPABKPSR006</t>
+  </si>
+  <si>
+    <t>10.214.0.4</t>
+  </si>
+  <si>
+    <t>CLPABKPSR007</t>
+  </si>
+  <si>
+    <t>clpabkpsr008</t>
+  </si>
+  <si>
+    <t>CLPABKPSR008</t>
+  </si>
+  <si>
+    <t>STP_AZU_DEV_CLPABKPSR004_GERAL_IndexServer</t>
+  </si>
+  <si>
+    <t>Serviço Commvault</t>
+  </si>
+  <si>
+    <t>STP_AZU_DEV_CLPABKPSR004_VM_IndexServer</t>
+  </si>
+  <si>
+    <t>STP_AZU_HLM_CLPABKPSR006_GERAL_IndexServer</t>
+  </si>
+  <si>
+    <t>STP_AZU_PRD_CLPABKPSR005_COLD_IndexServer</t>
+  </si>
+  <si>
+    <t>cmay21lb30</t>
+  </si>
+  <si>
+    <t>10.134.160.30</t>
+  </si>
+  <si>
+    <t>cmay21lb32</t>
+  </si>
+  <si>
+    <t>10.134.160.32</t>
+  </si>
+  <si>
+    <t>cmay22lb03</t>
+  </si>
+  <si>
+    <t>10.134.160.4</t>
+  </si>
+  <si>
+    <t>cmay22lb05</t>
+  </si>
+  <si>
+    <t>10.134.160.5</t>
+  </si>
+  <si>
+    <t>cmay22lb07</t>
+  </si>
+  <si>
+    <t>10.134.160.6</t>
+  </si>
+  <si>
+    <t>cmay22lb09</t>
+  </si>
+  <si>
+    <t>10.134.160.7</t>
+  </si>
+  <si>
+    <t>cmay22lb11</t>
+  </si>
+  <si>
+    <t>10.134.160.8</t>
+  </si>
+  <si>
+    <t>cmay22lb13</t>
+  </si>
+  <si>
+    <t>10.134.160.9</t>
+  </si>
+  <si>
+    <t>cmay22lb15</t>
+  </si>
+  <si>
+    <t>10.134.160.10</t>
+  </si>
+  <si>
+    <t>cmay22lb17</t>
+  </si>
+  <si>
+    <t>10.134.160.11</t>
+  </si>
+  <si>
+    <t>cmay22lb19</t>
+  </si>
+  <si>
+    <t>10.134.160.12</t>
+  </si>
+  <si>
+    <t>cmay22lb21</t>
+  </si>
+  <si>
+    <t>10.134.160.13</t>
+  </si>
+  <si>
+    <t>cmay22lb23</t>
+  </si>
+  <si>
+    <t>10.134.160.22</t>
+  </si>
+  <si>
+    <t>cmay22lb25</t>
+  </si>
+  <si>
+    <t>10.134.160.20</t>
+  </si>
+  <si>
+    <t>cmay22wb02</t>
+  </si>
+  <si>
+    <t>10.134.160.3</t>
+  </si>
+  <si>
+    <t>STP_DEDUP_CMAY22WB02_IndexServer</t>
+  </si>
+  <si>
+    <t>STP_NO_DEDUP_CMAY22TL29_IndexServer</t>
+  </si>
+  <si>
+    <t>SQLPROD01</t>
+  </si>
+  <si>
+    <t>10.1.1.114</t>
+  </si>
+  <si>
+    <t>SQLPROD02</t>
+  </si>
+  <si>
+    <t>10.1.1.115</t>
+  </si>
+  <si>
+    <t>SQLPROD03</t>
+  </si>
+  <si>
+    <t>10.1.1.116</t>
+  </si>
+  <si>
+    <t>SQLPROD04</t>
+  </si>
+  <si>
+    <t>10.1.1.117</t>
+  </si>
+  <si>
+    <t>SQLPROD11</t>
+  </si>
+  <si>
+    <t>10.1.1.128</t>
+  </si>
+  <si>
+    <t>SQLPROD12</t>
+  </si>
+  <si>
+    <t>10.1.1.129</t>
+  </si>
+  <si>
+    <t>SQLPROD13</t>
+  </si>
+  <si>
+    <t>10.1.1.112</t>
+  </si>
+  <si>
+    <t>brho11glo1014</t>
+  </si>
+  <si>
+    <t>10.37.25.156</t>
+  </si>
+  <si>
+    <t>brho11glo1029</t>
+  </si>
+  <si>
+    <t>10.37.25.196</t>
+  </si>
+  <si>
+    <t>brho11glo102c</t>
+  </si>
+  <si>
+    <t>10.37.24.73</t>
+  </si>
+  <si>
+    <t>brho11glo102e</t>
+  </si>
+  <si>
+    <t>10.37.24.155</t>
+  </si>
+  <si>
+    <t>brho11glo1042</t>
+  </si>
+  <si>
+    <t>10.37.25.176</t>
+  </si>
+  <si>
+    <t>CLPASQLSR002_AGClient</t>
+  </si>
+  <si>
+    <t>CLPASQLSR004_AGClient</t>
+  </si>
+  <si>
+    <t>CLPASQLSR006_AGClient</t>
+  </si>
+  <si>
+    <t>CMPASQLSR008_AGClient</t>
   </si>
 </sst>
 </file>
@@ -281,8 +659,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF600E73-FA71-484C-AF52-64E3E545EF77}" name="fileClient001" displayName="fileClient001" ref="A1:H18" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:H18" xr:uid="{CF600E73-FA71-484C-AF52-64E3E545EF77}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF600E73-FA71-484C-AF52-64E3E545EF77}" name="fileClient001" displayName="fileClient001" ref="A1:H87" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:H87" xr:uid="{CF600E73-FA71-484C-AF52-64E3E545EF77}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{43692159-A84C-4DF8-B837-27CB39407CCB}" uniqueName="1" name="Client" queryTableFieldId="1" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{AB5B074F-4A75-4F87-A7A7-0EC129B7451B}" uniqueName="2" name="Host Name" queryTableFieldId="2" dataDxfId="5"/>
@@ -594,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA384E93-0C43-4BD1-9E2D-AAE3DAA7EA6C}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A82" sqref="A82:H87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1076,6 +1454,1764 @@
         <v>18</v>
       </c>
       <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F50" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G50" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F53" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F54" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F55" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F59" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G60" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F61" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G61" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F62" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G62" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F63" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F64" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C66" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G66" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G67" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G68" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F83" s="1"/>
+      <c r="G83" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H87">
         <v>0</v>
       </c>
     </row>

</xml_diff>